<commit_message>
a bit more stuff
</commit_message>
<xml_diff>
--- a/Course Materials.xlsx
+++ b/Course Materials.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janke/Dropbox/satchel/projects/so-you-wanna-code/so-you-wanna-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2743FA1-56EF-AD46-8CCE-16B74AF0759E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B4B795-06E4-EC4F-96BD-D2595B8DEB70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="3820" windowWidth="14860" windowHeight="20560" xr2:uid="{FAFBAC99-EDA2-904A-8438-F3B9654B0E00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Books</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>Prices are per year</t>
+  </si>
+  <si>
+    <t>FastMail</t>
+  </si>
+  <si>
+    <t>Total with Optional Stuff</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192D7AE3-85A6-0C4A-BA14-7BD23C6FEA99}">
-  <dimension ref="B2:E49"/>
+  <dimension ref="B2:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,73 +792,78 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="D28" s="4">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="4">
-        <v>100</v>
-      </c>
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" s="4">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="D35" s="4"/>
+      <c r="E35" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="4">
+        <v>33</v>
+      </c>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C38" s="4"/>
@@ -863,12 +874,27 @@
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
+      <c r="B40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="4">
+        <f>SUM(C4:C38)</f>
+        <v>493</v>
+      </c>
+      <c r="D40" s="4">
+        <f>SUM(D4:D38)</f>
+        <v>682</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="4">
+        <f>C40+D40</f>
+        <v>1175</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C42" s="4"/>
@@ -879,40 +905,12 @@
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="4">
-        <f>SUM(C4:C42)</f>
-        <v>493</v>
-      </c>
-      <c r="D44" s="4">
-        <f>SUM(D4:D41)</f>
-        <v>646</v>
-      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C45" s="4"/>
-      <c r="D45" s="4">
-        <f>C44+D44</f>
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
+      <c r="D45" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>